<commit_message>
put pdf in one page
</commit_message>
<xml_diff>
--- a/POPC/MATRIX/Workbook1.xlsx
+++ b/POPC/MATRIX/Workbook1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
-  <workbookPr showInkAnnotation="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ali/Google Drive/MacBook Air/sem2/ProgAlgo/Labs/lab2/ProgAlg-labo002/project/ProgAlg-Lab2/POPC/MATRIX/"/>
@@ -60,7 +60,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,31 +69,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
+      <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Consolas"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="16"/>
+      <sz val="11"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
@@ -118,9 +125,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -129,16 +136,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -190,7 +194,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$34</c:f>
+              <c:f>Sheet1!$B$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -219,7 +223,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$35:$C$39</c:f>
+              <c:f>Sheet1!$B$52:$B$56</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -248,7 +252,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$34</c:f>
+              <c:f>Sheet1!$C$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -277,7 +281,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$35:$D$39</c:f>
+              <c:f>Sheet1!$C$52:$C$56</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -306,7 +310,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$34</c:f>
+              <c:f>Sheet1!$D$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -335,7 +339,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$35:$E$39</c:f>
+              <c:f>Sheet1!$D$52:$D$56</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1105,14 +1109,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1308100</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1400,31 +1404,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" style="4" customWidth="1"/>
-    <col min="10" max="16" width="10.83203125" style="4"/>
-    <col min="17" max="17" width="13.6640625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="15" style="4" customWidth="1"/>
-    <col min="20" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="2" width="8.6640625" style="4"/>
+    <col min="3" max="3" width="7.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1451,7 +1445,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1483,7 +1477,7 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1516,7 +1510,7 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1549,7 +1543,7 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1582,7 +1576,7 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1615,32 +1609,32 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:15" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>6240</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>10</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>5</v>
       </c>
-      <c r="E7" s="6">
-        <v>2</v>
-      </c>
-      <c r="F7" s="6">
-        <v>4</v>
-      </c>
-      <c r="G7" s="6">
+      <c r="E7" s="5">
+        <v>2</v>
+      </c>
+      <c r="F7" s="5">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5">
         <v>10.276</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>17.899999999999999</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>24.06</v>
       </c>
       <c r="K7" s="5"/>
@@ -1648,7 +1642,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1677,7 +1671,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -1706,7 +1700,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -1735,7 +1729,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -1764,7 +1758,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -1793,36 +1787,36 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="20" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>4620</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>9</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>3</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>3</v>
       </c>
-      <c r="F13" s="6">
-        <v>4</v>
-      </c>
-      <c r="G13" s="6">
+      <c r="F13" s="5">
+        <v>4</v>
+      </c>
+      <c r="G13" s="5">
         <v>7.87</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>8.3719999999999999</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="5">
         <v>10.94</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -1851,7 +1845,7 @@
         <v>5.72</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -1880,7 +1874,7 @@
         <v>5.72</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -1909,7 +1903,7 @@
         <v>5.74</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>4</v>
       </c>
@@ -1938,7 +1932,7 @@
         <v>5.73</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>5</v>
       </c>
@@ -1967,36 +1961,36 @@
         <v>5.74</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="20" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>3240</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>6</v>
       </c>
-      <c r="D19" s="6">
-        <v>2</v>
-      </c>
-      <c r="E19" s="6">
+      <c r="D19" s="5">
+        <v>2</v>
+      </c>
+      <c r="E19" s="5">
         <v>3</v>
       </c>
-      <c r="F19" s="6">
-        <v>4</v>
-      </c>
-      <c r="G19" s="6">
+      <c r="F19" s="5">
+        <v>4</v>
+      </c>
+      <c r="G19" s="5">
         <v>5.7519999999999998</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <v>3.3279999999999998</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="5">
         <v>5.73</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -2025,7 +2019,7 @@
         <v>2.63</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2</v>
       </c>
@@ -2054,7 +2048,7 @@
         <v>2.62</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>3</v>
       </c>
@@ -2083,7 +2077,7 @@
         <v>2.63</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>4</v>
       </c>
@@ -2112,7 +2106,7 @@
         <v>2.61</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>5</v>
       </c>
@@ -2141,36 +2135,36 @@
         <v>2.63</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="20" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>2160</v>
       </c>
-      <c r="C25" s="6">
-        <v>4</v>
-      </c>
-      <c r="D25" s="6">
-        <v>2</v>
-      </c>
-      <c r="E25" s="6">
-        <v>2</v>
-      </c>
-      <c r="F25" s="6">
-        <v>4</v>
-      </c>
-      <c r="G25" s="6">
+      <c r="C25" s="5">
+        <v>4</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2</v>
+      </c>
+      <c r="E25" s="5">
+        <v>2</v>
+      </c>
+      <c r="F25" s="5">
+        <v>4</v>
+      </c>
+      <c r="G25" s="5">
         <v>2.6080000000000001</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="5">
         <v>1.1779999999999999</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="5">
         <v>2.6240000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -2199,7 +2193,7 @@
         <v>0.66500000000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2</v>
       </c>
@@ -2228,7 +2222,7 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>3</v>
       </c>
@@ -2257,7 +2251,7 @@
         <v>0.71699999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>4</v>
       </c>
@@ -2286,7 +2280,7 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>5</v>
       </c>
@@ -2315,121 +2309,123 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="20" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>1080</v>
       </c>
-      <c r="C31" s="6">
-        <v>2</v>
-      </c>
-      <c r="D31" s="6">
+      <c r="C31" s="5">
+        <v>2</v>
+      </c>
+      <c r="D31" s="5">
         <v>1</v>
       </c>
-      <c r="E31" s="6">
-        <v>2</v>
-      </c>
-      <c r="F31" s="6">
-        <v>4</v>
-      </c>
-      <c r="G31" s="6">
+      <c r="E31" s="5">
+        <v>2</v>
+      </c>
+      <c r="F31" s="5">
+        <v>4</v>
+      </c>
+      <c r="G31" s="5">
         <v>1.27</v>
       </c>
-      <c r="H31" s="6">
+      <c r="H31" s="5">
         <v>0.314</v>
       </c>
-      <c r="I31" s="6">
+      <c r="I31" s="5">
         <v>0.83760000000000001</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="23" x14ac:dyDescent="0.3">
-      <c r="B34" s="2" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B35" s="5">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
         <v>6240</v>
       </c>
-      <c r="C35" s="7">
+      <c r="B52" s="6">
         <v>10.276</v>
       </c>
-      <c r="D35" s="7">
+      <c r="C52" s="6">
         <v>17.899999999999999</v>
       </c>
-      <c r="E35" s="7">
+      <c r="D52" s="6">
         <v>24.06</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B36" s="5">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
         <v>4620</v>
       </c>
-      <c r="C36" s="7">
+      <c r="B53" s="6">
         <v>7.87</v>
       </c>
-      <c r="D36" s="7">
+      <c r="C53" s="6">
         <v>8.3719999999999999</v>
       </c>
-      <c r="E36" s="7">
+      <c r="D53" s="6">
         <v>10.94</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B37" s="5">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
         <v>3240</v>
       </c>
-      <c r="C37" s="7">
+      <c r="B54" s="6">
         <v>5.7519999999999998</v>
       </c>
-      <c r="D37" s="7">
+      <c r="C54" s="6">
         <v>3.3279999999999998</v>
       </c>
-      <c r="E37" s="7">
+      <c r="D54" s="6">
         <v>5.73</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B38" s="5">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
         <v>2160</v>
       </c>
-      <c r="C38" s="7">
+      <c r="B55" s="6">
         <v>2.6080000000000001</v>
       </c>
-      <c r="D38" s="7">
+      <c r="C55" s="6">
         <v>1.1779999999999999</v>
       </c>
-      <c r="E38" s="7">
+      <c r="D55" s="6">
         <v>2.6240000000000001</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B39" s="5">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="5">
         <v>1080</v>
       </c>
-      <c r="C39" s="7">
+      <c r="B56" s="6">
         <v>1.27</v>
       </c>
-      <c r="D39" s="7">
+      <c r="C56" s="6">
         <v>0.314</v>
       </c>
-      <c r="E39" s="7">
+      <c r="D56" s="6">
         <v>0.83760000000000001</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>